<commit_message>
forbedred parametergenerering og lagt inn nye tall
</commit_message>
<xml_diff>
--- a/data_generation/SetData-sheets.xlsx
+++ b/data_generation/SetData-sheets.xlsx
@@ -6471,7 +6471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6509,6 +6509,11 @@
     <row r="6">
       <c r="A6" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6558,7 +6563,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6588,6 +6593,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6599,7 +6609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6647,6 +6657,16 @@
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6776,7 +6796,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A101"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6836,461 +6856,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>100</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>